<commit_message>
new profile details added in excel file
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24701"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{392EF910-14FB-468F-93B4-8A3991425A34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66EA4C77-6F49-4D66-8AF6-BDD927C3AEF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RUNMANAGER" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="57">
   <si>
     <t>testname</t>
   </si>
@@ -129,21 +129,9 @@
     <t>VGhyaW5hdGhAMTk5Nw==</t>
   </si>
   <si>
-    <t>thrinath.k03@outlook.com</t>
-  </si>
-  <si>
     <t>112.0.5615.138</t>
   </si>
   <si>
-    <t>sivalewi@gmail.com</t>
-  </si>
-  <si>
-    <t>U2l2YUAxODE0</t>
-  </si>
-  <si>
-    <t>D:\\C_Siva_Sankar_Resume_Nw.pdf</t>
-  </si>
-  <si>
     <t>S2lyYW5AMTMxNw==</t>
   </si>
   <si>
@@ -162,9 +150,6 @@
     <t>D:\\CS_Sankar_QA.pdf</t>
   </si>
   <si>
-    <t>D:\\Thrinath_K.pdf</t>
-  </si>
-  <si>
     <t>VGhhbmt5b3VANTA=</t>
   </si>
   <si>
@@ -175,6 +160,33 @@
   </si>
   <si>
     <t>no</t>
+  </si>
+  <si>
+    <t>112.0.5615</t>
+  </si>
+  <si>
+    <t>VmFyYUAxMjM=</t>
+  </si>
+  <si>
+    <t>kvaralakshmi741@gmail.com</t>
+  </si>
+  <si>
+    <t>D:\\Varalakshmi_K.pdf</t>
+  </si>
+  <si>
+    <t>D:\\Sandeep_Resume.pdf</t>
+  </si>
+  <si>
+    <t>sandeep.venkata19@gmail.com</t>
+  </si>
+  <si>
+    <t>U2FuZHlAMTk5MQ==</t>
+  </si>
+  <si>
+    <t>thrinathk03@gmail.com</t>
+  </si>
+  <si>
+    <t>D:\\K_Thrinath_QA.pdf</t>
   </si>
 </sst>
 </file>
@@ -581,7 +593,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -619,7 +631,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>10</v>
@@ -636,7 +648,7 @@
         <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>11</v>
@@ -653,7 +665,7 @@
         <v>25</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>10</v>
@@ -687,10 +699,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -952,7 +964,7 @@
         <v>33</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>36</v>
@@ -961,7 +973,7 @@
         <v>16</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
@@ -975,19 +987,19 @@
         <v>22</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>53</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>16</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
@@ -1001,19 +1013,19 @@
         <v>22</v>
       </c>
       <c r="D12" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E12" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>42</v>
-      </c>
       <c r="G12" s="3" t="s">
         <v>16</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
@@ -1021,25 +1033,25 @@
         <v>34</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>9</v>
+        <v>47</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>16</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
@@ -1047,25 +1059,51 @@
         <v>34</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>9</v>
+        <v>47</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E14" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A15" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H15" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1076,8 +1114,9 @@
     <hyperlink ref="E12" r:id="rId4" xr:uid="{BCD26498-8ACE-4EBF-8E09-36A0718FFD27}"/>
     <hyperlink ref="E13" r:id="rId5" xr:uid="{0A1BCAC4-567E-4AEE-9CFE-31770699C913}"/>
     <hyperlink ref="E14" r:id="rId6" xr:uid="{6649E398-EE93-427C-9209-BBB0546BABE6}"/>
+    <hyperlink ref="E15" r:id="rId7" xr:uid="{1C2ADAAF-5533-4A3E-8B51-B0F467D05247}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId7"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
resumes data added in newly created resume folder
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24701"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8DADBCC-0CAB-4B2D-BB92-C461D852F3A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E64C23D5-22EB-4CD7-A5B0-EEB2FA598A59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -132,15 +132,6 @@
     <t>112.0.5615.138</t>
   </si>
   <si>
-    <t>S2lyYW5AMTMxNw==</t>
-  </si>
-  <si>
-    <t>hemakiran131722@gmail.com</t>
-  </si>
-  <si>
-    <t>D:\\Resume-2.pdf</t>
-  </si>
-  <si>
     <t>U2l2YUAxOTk5</t>
   </si>
   <si>
@@ -186,9 +177,6 @@
     <t>thrinathk03@gmail.com</t>
   </si>
   <si>
-    <t>D:\\K_Thrinath_QA.pdf</t>
-  </si>
-  <si>
     <t>R2FuZXNoQDEyMzQ=</t>
   </si>
   <si>
@@ -196,6 +184,18 @@
   </si>
   <si>
     <t>D:\\Naresh_Resume.pdf</t>
+  </si>
+  <si>
+    <t>D:\\K_Thrinath.docx</t>
+  </si>
+  <si>
+    <t>udaylewi@gmail.com</t>
+  </si>
+  <si>
+    <t>VWRheUA4MDc0</t>
+  </si>
+  <si>
+    <t>D:\\Uday_Resume.docx</t>
   </si>
 </sst>
 </file>
@@ -640,7 +640,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>10</v>
@@ -657,7 +657,7 @@
         <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>11</v>
@@ -674,7 +674,7 @@
         <v>25</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>10</v>
@@ -710,8 +710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -973,7 +973,7 @@
         <v>33</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>36</v>
@@ -999,16 +999,16 @@
         <v>37</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>16</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
@@ -1016,7 +1016,7 @@
         <v>34</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>47</v>
+        <v>9</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>22</v>
@@ -1025,16 +1025,16 @@
         <v>37</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>16</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
@@ -1042,7 +1042,7 @@
         <v>34</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>22</v>
@@ -1051,16 +1051,16 @@
         <v>37</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>16</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
@@ -1068,7 +1068,7 @@
         <v>34</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>22</v>
@@ -1077,16 +1077,16 @@
         <v>37</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>16</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
@@ -1094,25 +1094,25 @@
         <v>34</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D15" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H15" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
@@ -1126,19 +1126,19 @@
         <v>22</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>16</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
testdata excel data update
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24701"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E64C23D5-22EB-4CD7-A5B0-EEB2FA598A59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C7E37F4-AB11-42D4-B6ED-2501668A5992}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -165,9 +165,6 @@
     <t>D:\\Varalakshmi_K.pdf</t>
   </si>
   <si>
-    <t>D:\\Sandeep_Resume.pdf</t>
-  </si>
-  <si>
     <t>sandeep.venkata19@gmail.com</t>
   </si>
   <si>
@@ -183,19 +180,22 @@
     <t>nareshbabuind7@gmail.com</t>
   </si>
   <si>
-    <t>D:\\Naresh_Resume.pdf</t>
-  </si>
-  <si>
-    <t>D:\\K_Thrinath.docx</t>
-  </si>
-  <si>
     <t>udaylewi@gmail.com</t>
   </si>
   <si>
     <t>VWRheUA4MDc0</t>
   </si>
   <si>
-    <t>D:\\Uday_Resume.docx</t>
+    <t>./resume/K_Thrinath.docx</t>
+  </si>
+  <si>
+    <t>./resume/Sandeep_Resume.pdf</t>
+  </si>
+  <si>
+    <t>./resume/Uday_Resume.docx</t>
+  </si>
+  <si>
+    <t>./resume/Naresh_Resume.pdf</t>
   </si>
 </sst>
 </file>
@@ -711,7 +711,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -973,7 +973,7 @@
         <v>33</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>36</v>
@@ -981,7 +981,7 @@
       <c r="G10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="H10" s="2" t="s">
         <v>56</v>
       </c>
     </row>
@@ -999,16 +999,16 @@
         <v>37</v>
       </c>
       <c r="E11" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>51</v>
-      </c>
       <c r="G11" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H11" s="1" t="s">
-        <v>49</v>
+      <c r="H11" s="2" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
@@ -1025,16 +1025,16 @@
         <v>37</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F12" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12" s="2" t="s">
         <v>58</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
@@ -1129,16 +1129,16 @@
         <v>45</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H16" s="1" t="s">
-        <v>55</v>
+      <c r="H16" s="2" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new test added to save resume headline
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24701"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C7E37F4-AB11-42D4-B6ED-2501668A5992}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18DF36D8-7168-4B96-89F7-E933A895E6C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -186,16 +186,16 @@
     <t>VWRheUA4MDc0</t>
   </si>
   <si>
-    <t>./resume/K_Thrinath.docx</t>
-  </si>
-  <si>
-    <t>./resume/Sandeep_Resume.pdf</t>
-  </si>
-  <si>
-    <t>./resume/Uday_Resume.docx</t>
-  </si>
-  <si>
-    <t>./resume/Naresh_Resume.pdf</t>
+    <t>D:\\Naresh_Resume.pdf</t>
+  </si>
+  <si>
+    <t>D:\\K_Thrinath.docx</t>
+  </si>
+  <si>
+    <t>D:\\Sandeep_Resume.pdf</t>
+  </si>
+  <si>
+    <t>D:\\Uday_Resume.docx</t>
   </si>
 </sst>
 </file>
@@ -982,7 +982,7 @@
         <v>16</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
@@ -1008,7 +1008,7 @@
         <v>16</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
@@ -1034,7 +1034,7 @@
         <v>16</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
@@ -1138,7 +1138,7 @@
         <v>16</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new block of code added to get day of the profile updated
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24701"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18DF36D8-7168-4B96-89F7-E933A895E6C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{918BCC47-219C-4E4D-B141-DDA600D4595E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -711,7 +711,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1120,7 +1120,7 @@
         <v>34</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>22</v>

</xml_diff>